<commit_message>
create api controlers for get tours, types of tours
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progect\Muhina\task_12_avalonia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DAC4CC-2D7D-4E22-A0DA-6974C053E76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E118D81-4116-49D6-85C4-07801623EF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Требование</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>метод для проверки подключения к базе данных</t>
+  </si>
+  <si>
+    <t>релизован метод для получения типов туров для соритровки</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +532,7 @@
     <col min="1" max="1" width="93.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -537,270 +540,435 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>48</v>
+      <c r="C48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B51">
-        <f>SUM(B2:B46)</f>
-        <v>3</v>
-      </c>
-      <c r="C51">
-        <v>43</v>
+      <c r="B52">
+        <f>SUM(B2:B51)</f>
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <f>SUM(C2:C51)</f>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
crocess creating tour page
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progect\Muhina\task_12_avalonia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ЧерновСВ\source\repos\tour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3702690D-B456-454C-B174-89A45FC5A255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C42FB5-478C-46CD-91C9-7E16888C14A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Требование</t>
   </si>
@@ -177,12 +177,6 @@
     <t>составить readme файл</t>
   </si>
   <si>
-    <t>сообзения об ошибках пользовалетя</t>
-  </si>
-  <si>
-    <t>подтверждение создания/редактирования/удаления</t>
-  </si>
-  <si>
     <t>сообщение пользователю о сохранении, удалении, изменении</t>
   </si>
   <si>
@@ -195,13 +189,7 @@
     <t>релизован метод для получения типов туров для соритровки</t>
   </si>
   <si>
-    <t>не возможно - нет связи базы данных</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>не возможно - нет колонки</t>
+    <t>подтверждение удаления</t>
   </si>
 </sst>
 </file>
@@ -530,16 +518,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="93.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,7 +562,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -596,7 +584,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -653,8 +641,8 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
-        <v>53</v>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -664,8 +652,8 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
-        <v>55</v>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -686,6 +674,9 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
       <c r="C14">
         <v>1</v>
       </c>
@@ -884,8 +875,8 @@
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B38" t="s">
-        <v>53</v>
+      <c r="B38">
+        <v>1</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -895,8 +886,8 @@
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" t="s">
-        <v>53</v>
+      <c r="B39">
+        <v>1</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -967,54 +958,52 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="2"/>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B52">
         <f>SUM(B2:B51)</f>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C52">
         <f>SUM(C2:C51)</f>
         <v>50</v>
-      </c>
-      <c r="D52" t="s">
-        <v>54</v>
-      </c>
-      <c r="E52">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create counter hotels page
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progect\Muhina\tour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412B6B93-4AF2-4AA8-95E3-1F4D0A4A7439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626DA9C0-2B08-45A5-8D8F-950ECD948070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,6 +715,9 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
       <c r="C18">
         <v>1</v>
       </c>
@@ -723,6 +726,9 @@
       <c r="A19" t="s">
         <v>16</v>
       </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
       <c r="C19">
         <v>1</v>
       </c>
@@ -731,6 +737,9 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
       <c r="C20">
         <v>1</v>
       </c>
@@ -747,6 +756,9 @@
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
       <c r="C22">
         <v>1</v>
       </c>
@@ -755,6 +767,9 @@
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
       <c r="C23">
         <v>1</v>
       </c>
@@ -763,6 +778,9 @@
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
       <c r="C24">
         <v>1</v>
       </c>
@@ -804,6 +822,9 @@
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
       <c r="C28">
         <v>1</v>
       </c>
@@ -812,6 +833,9 @@
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
       <c r="C29">
         <v>1</v>
       </c>
@@ -820,6 +844,9 @@
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
       <c r="C30">
         <v>1</v>
       </c>
@@ -828,6 +855,9 @@
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
       <c r="C31">
         <v>1</v>
       </c>
@@ -836,6 +866,9 @@
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
       <c r="C32">
         <v>1</v>
       </c>
@@ -979,6 +1012,9 @@
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
       <c r="C49">
         <v>1</v>
       </c>
@@ -998,6 +1034,9 @@
       <c r="A51" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
       <c r="C51">
         <v>1</v>
       </c>
@@ -1008,7 +1047,7 @@
       </c>
       <c r="B52">
         <f>SUM(B2:B51)</f>
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C52">
         <f>SUM(C2:C51)</f>

</xml_diff>

<commit_message>
update algorytms and create styles
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progect\Muhina\tour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626DA9C0-2B08-45A5-8D8F-950ECD948070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBB20E6-70C5-4978-8613-8A4A504D2664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,6 +707,9 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
       <c r="C17">
         <v>1</v>
       </c>
@@ -748,6 +751,9 @@
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
       <c r="C21">
         <v>1</v>
       </c>
@@ -877,6 +883,9 @@
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
       <c r="C33">
         <v>1</v>
       </c>
@@ -885,6 +894,9 @@
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
       <c r="C34">
         <v>1</v>
       </c>
@@ -893,6 +905,9 @@
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
       <c r="C35">
         <v>1</v>
       </c>
@@ -901,6 +916,9 @@
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
       <c r="C36">
         <v>1</v>
       </c>
@@ -909,6 +927,9 @@
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
       <c r="C37">
         <v>1</v>
       </c>
@@ -939,6 +960,9 @@
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
       <c r="C40">
         <v>1</v>
       </c>
@@ -947,6 +971,9 @@
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
       <c r="C41">
         <v>1</v>
       </c>
@@ -955,6 +982,9 @@
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
       <c r="C42">
         <v>1</v>
       </c>
@@ -963,6 +993,9 @@
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
       <c r="C43">
         <v>1</v>
       </c>
@@ -971,6 +1004,9 @@
       <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
       <c r="C44">
         <v>1</v>
       </c>
@@ -979,6 +1015,9 @@
       <c r="A45" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
       <c r="C45">
         <v>1</v>
       </c>
@@ -987,6 +1026,9 @@
       <c r="A46" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
       <c r="C46">
         <v>1</v>
       </c>
@@ -995,6 +1037,9 @@
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
       <c r="C47">
         <v>1</v>
       </c>
@@ -1047,7 +1092,7 @@
       </c>
       <c r="B52">
         <f>SUM(B2:B51)</f>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C52">
         <f>SUM(C2:C51)</f>

</xml_diff>